<commit_message>
A lot of things
</commit_message>
<xml_diff>
--- a/sdfsd.xlsx
+++ b/sdfsd.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>קוד קופון</t>
   </si>
@@ -40,16 +40,19 @@
     <t>סטטוס</t>
   </si>
   <si>
-    <t>115000386-9340</t>
-  </si>
-  <si>
-    <t>FreeFit</t>
-  </si>
-  <si>
-    <t>שובר בשווי 200 ₪</t>
-  </si>
-  <si>
-    <t>הנחה</t>
+    <t>להלה</t>
+  </si>
+  <si>
+    <t>Love Gift Card</t>
+  </si>
+  <si>
+    <t>שובר בסך 100 ש"ח</t>
+  </si>
+  <si>
+    <t>2023-10-31</t>
+  </si>
+  <si>
+    <t>מבצע</t>
   </si>
   <si>
     <t>פעיל</t>
@@ -447,10 +450,10 @@
         <v>8</v>
       </c>
       <c r="B2">
-        <v>200</v>
+        <v>100</v>
       </c>
       <c r="C2">
-        <v>160</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
         <v>9</v>
@@ -458,11 +461,14 @@
       <c r="E2" t="s">
         <v>10</v>
       </c>
+      <c r="F2" t="s">
+        <v>11</v>
+      </c>
       <c r="G2" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="H2" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>